<commit_message>
changed data filling folder
</commit_message>
<xml_diff>
--- a/Final Report.xlsx
+++ b/Final Report.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="My Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,117 +426,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>From</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>To</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Query</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sheet</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2020-08-25 00:00:00</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2020-08-26 00:00:00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Stats with filter</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>{'created_date': {'$gte': datetime.datetime(2020, 8, 25, 0, 0), '$lt': datetime.datetime(2020, 8, 26, 0, 0)}, 'client_id': 'MNRNJVXE', 'function_name': {'$eq': 'authorize'}, 'user_id': {'$ne': None}}</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>My Sheet</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2020-10-06 00:00:00</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2020-10-07 00:00:00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sarvi with filter</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>{'created_date': {'$gte': datetime.datetime(2020, 10, 6, 0, 0), '$lt': datetime.datetime(2020, 10, 7, 0, 0)}, 'client_id': 'MNRNJVXE', 'function_name': {'$ne': 'authorize'}, 'user_id': {'$ne': None}}</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>My Sheet</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -582,22 +469,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-08-25 00:00:00</t>
+          <t>2020-10-06 00:00:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2020-08-26 00:00:00</t>
+          <t>2020-10-07 00:00:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Stats for Date Range</t>
+          <t>sarvi with filter</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'created_date': {'$gte': datetime.datetime(2020, 8, 25, 0, 0), '$lt': datetime.datetime(2020, 8, 26, 0, 0)}, 'client_id': 'MNRNJVXE', 'function_name': {'$eq': 'authorize'}, 'user_id': {'$ne': True}}</t>
+          <t>{'created_date': {'$gte': datetime.datetime(2020, 10, 6, 0, 0), '$lt': datetime.datetime(2020, 10, 7, 0, 0)}, 'client_id': 'MNRNJVXE', 'function_name': {'$ne': 'authorize'}, 'user_id': {'$ne': None}}</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -605,88 +492,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Main</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>From</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>To</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Query</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sheet</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2020-10-06 00:00:00</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2020-10-07 00:00:00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Function Name Filter</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>{'created_date': {'$gte': datetime.datetime(2020, 10, 6, 0, 0), '$lt': datetime.datetime(2020, 10, 7, 0, 0)}, 'client_id': 'MNRNJVXE', 'function_name': {'$eq': 'authorize'}, 'user_id': {'$ne': None}}</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Sheet 1</t>
+          <t>My Sheet</t>
         </is>
       </c>
     </row>

</xml_diff>